<commit_message>
no rest for the weary
</commit_message>
<xml_diff>
--- a/grades.xlsx
+++ b/grades.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alf\Desktop\x86\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07E9A702-A5E1-4C89-8BFA-E6591EEB7F28}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A01A1E36-3EB2-45F4-968B-DB9A196D1043}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="7680" windowHeight="2580" xr2:uid="{BEB47269-8309-432F-A838-264E8E734028}"/>
   </bookViews>
@@ -627,7 +627,7 @@
   <dimension ref="A2:AC27"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -827,7 +827,7 @@
       <c r="C5" s="13"/>
       <c r="D5" s="10">
         <f>D6*D2</f>
-        <v>1.7475728155339806E-2</v>
+        <v>2.2330097087378643E-2</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>14</v>
@@ -836,7 +836,7 @@
       <c r="H5" s="13"/>
       <c r="I5" s="10">
         <f>I6*I2</f>
-        <v>8.0000000000000002E-3</v>
+        <v>1.6E-2</v>
       </c>
       <c r="K5" s="5" t="s">
         <v>14</v>
@@ -845,7 +845,7 @@
       <c r="M5" s="13"/>
       <c r="N5" s="10">
         <f>N6*N2</f>
-        <v>0</v>
+        <v>4.2477876106194697E-2</v>
       </c>
       <c r="P5" s="5" t="s">
         <v>14</v>
@@ -872,7 +872,7 @@
       <c r="AB5" s="13"/>
       <c r="AC5" s="10">
         <f>D5+I5+N5+S5+X5</f>
-        <v>2.5475728155339807E-2</v>
+        <v>8.0807973193573329E-2</v>
       </c>
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.25">
@@ -881,7 +881,7 @@
       </c>
       <c r="B6" s="8">
         <f>SUM(B7:B27)</f>
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="C6" s="8">
         <f>SUM(C7:C27)</f>
@@ -889,14 +889,14 @@
       </c>
       <c r="D6" s="9">
         <f>IF(C6&lt;&gt;0,B6/C6,0)</f>
-        <v>0.17475728155339806</v>
+        <v>0.22330097087378642</v>
       </c>
       <c r="F6" s="5" t="s">
         <v>13</v>
       </c>
       <c r="G6" s="8">
         <f>SUM(G7:G16)</f>
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="H6" s="8">
         <f>SUM(H7:H16)</f>
@@ -904,14 +904,14 @@
       </c>
       <c r="I6" s="9">
         <f>IF(H6&lt;&gt;0,G6/H6,0)</f>
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="K6" s="5" t="s">
         <v>13</v>
       </c>
       <c r="L6" s="8">
         <f>SUM(L7:L14)</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="M6" s="8">
         <f>SUM(M7:M14)</f>
@@ -919,7 +919,7 @@
       </c>
       <c r="N6" s="9">
         <f>IF(M6&lt;&gt;0,L6/M6,0)</f>
-        <v>0</v>
+        <v>0.13274336283185842</v>
       </c>
       <c r="P6" s="5" t="s">
         <v>13</v>
@@ -969,24 +969,28 @@
       <c r="F7" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="G7" s="8"/>
+      <c r="G7" s="8">
+        <v>20</v>
+      </c>
       <c r="H7" s="8">
         <v>20</v>
       </c>
       <c r="I7" s="9">
         <f t="shared" ref="I7" si="1">IF(H7&lt;&gt;0,G7/H7,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K7" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="L7" s="8"/>
+      <c r="L7" s="8">
+        <v>15</v>
+      </c>
       <c r="M7" s="8">
         <v>15</v>
       </c>
       <c r="N7" s="9">
         <f t="shared" ref="N7" si="2">IF(M7&lt;&gt;0,L7/M7,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P7" s="3" t="s">
         <v>50</v>
@@ -1351,13 +1355,15 @@
       <c r="A18" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="8"/>
+      <c r="B18" s="8">
+        <v>10</v>
+      </c>
       <c r="C18" s="8">
         <v>10</v>
       </c>
       <c r="D18" s="9">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Ruby is not a systems programming language
So what the hell am I doing??
</commit_message>
<xml_diff>
--- a/grades.xlsx
+++ b/grades.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alf\Desktop\x86\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A01A1E36-3EB2-45F4-968B-DB9A196D1043}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3468964-367C-4276-A0BB-3D97B7E08427}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="7680" windowHeight="2580" xr2:uid="{BEB47269-8309-432F-A838-264E8E734028}"/>
   </bookViews>
@@ -627,7 +627,7 @@
   <dimension ref="A2:AC27"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
more to come tomorrow
</commit_message>
<xml_diff>
--- a/grades.xlsx
+++ b/grades.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alf\Desktop\x86\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3468964-367C-4276-A0BB-3D97B7E08427}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EC9A6D2-9616-423B-A81B-DBE2ECA2CF60}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="7680" windowHeight="2580" xr2:uid="{BEB47269-8309-432F-A838-264E8E734028}"/>
   </bookViews>
@@ -627,7 +627,7 @@
   <dimension ref="A2:AC27"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -827,7 +827,7 @@
       <c r="C5" s="13"/>
       <c r="D5" s="10">
         <f>D6*D2</f>
-        <v>2.2330097087378643E-2</v>
+        <v>1.7475728155339806E-2</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>14</v>
@@ -872,7 +872,7 @@
       <c r="AB5" s="13"/>
       <c r="AC5" s="10">
         <f>D5+I5+N5+S5+X5</f>
-        <v>8.0807973193573329E-2</v>
+        <v>7.5953604261534496E-2</v>
       </c>
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.25">
@@ -881,7 +881,7 @@
       </c>
       <c r="B6" s="8">
         <f>SUM(B7:B27)</f>
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="C6" s="8">
         <f>SUM(C7:C27)</f>
@@ -889,7 +889,7 @@
       </c>
       <c r="D6" s="9">
         <f>IF(C6&lt;&gt;0,B6/C6,0)</f>
-        <v>0.22330097087378642</v>
+        <v>0.17475728155339806</v>
       </c>
       <c r="F6" s="5" t="s">
         <v>13</v>
@@ -1080,15 +1080,13 @@
       <c r="A9" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="8">
-        <v>10</v>
-      </c>
+      <c r="B9" s="8"/>
       <c r="C9" s="8">
         <v>10</v>
       </c>
       <c r="D9" s="9">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>32</v>

</xml_diff>

<commit_message>
f e w f
cinnamon bun required.
</commit_message>
<xml_diff>
--- a/grades.xlsx
+++ b/grades.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alf\Desktop\x86\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EC9A6D2-9616-423B-A81B-DBE2ECA2CF60}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B593A271-D0EE-4042-9D1A-2A739844CC70}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="7680" windowHeight="2580" xr2:uid="{BEB47269-8309-432F-A838-264E8E734028}"/>
   </bookViews>
@@ -627,7 +627,7 @@
   <dimension ref="A2:AC27"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -827,7 +827,7 @@
       <c r="C5" s="13"/>
       <c r="D5" s="10">
         <f>D6*D2</f>
-        <v>1.7475728155339806E-2</v>
+        <v>2.7184466019417475E-2</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>14</v>
@@ -872,7 +872,7 @@
       <c r="AB5" s="13"/>
       <c r="AC5" s="10">
         <f>D5+I5+N5+S5+X5</f>
-        <v>7.5953604261534496E-2</v>
+        <v>8.5662342125612162E-2</v>
       </c>
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.25">
@@ -881,7 +881,7 @@
       </c>
       <c r="B6" s="8">
         <f>SUM(B7:B27)</f>
-        <v>36</v>
+        <v>56</v>
       </c>
       <c r="C6" s="8">
         <f>SUM(C7:C27)</f>
@@ -889,7 +889,7 @@
       </c>
       <c r="D6" s="9">
         <f>IF(C6&lt;&gt;0,B6/C6,0)</f>
-        <v>0.17475728155339806</v>
+        <v>0.27184466019417475</v>
       </c>
       <c r="F6" s="5" t="s">
         <v>13</v>
@@ -1080,13 +1080,15 @@
       <c r="A9" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="8"/>
+      <c r="B9" s="8">
+        <v>10</v>
+      </c>
       <c r="C9" s="8">
         <v>10</v>
       </c>
       <c r="D9" s="9">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>32</v>
@@ -1115,13 +1117,15 @@
       <c r="A10" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="8"/>
+      <c r="B10" s="8">
+        <v>10</v>
+      </c>
       <c r="C10" s="8">
         <v>10</v>
       </c>
       <c r="D10" s="9">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>33</v>

</xml_diff>

<commit_message>
homework 4 is fun!
My first loop in assembly!
Okay maybe not my first loop but my first loop in like two years.
</commit_message>
<xml_diff>
--- a/grades.xlsx
+++ b/grades.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alf\Desktop\x86\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E54E8808-B025-40B4-AF65-BD3A11F136CD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8069FD3-BCEE-4586-8BC5-865FCDE1C0F0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="7680" windowHeight="2580" xr2:uid="{BEB47269-8309-432F-A838-264E8E734028}"/>
   </bookViews>
@@ -627,7 +627,7 @@
   <dimension ref="A2:AC27"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -845,7 +845,7 @@
       <c r="M5" s="13"/>
       <c r="N5" s="10">
         <f>N6*N2</f>
-        <v>4.2477876106194697E-2</v>
+        <v>7.9292035398230085E-2</v>
       </c>
       <c r="P5" s="5" t="s">
         <v>14</v>
@@ -872,7 +872,7 @@
       <c r="AB5" s="13"/>
       <c r="AC5" s="10">
         <f>D5+I5+N5+S5+X5</f>
-        <v>0.10022544892172869</v>
+        <v>0.13703960821376407</v>
       </c>
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.25">
@@ -911,7 +911,7 @@
       </c>
       <c r="L6" s="8">
         <f>SUM(L7:L14)</f>
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="M6" s="8">
         <f>SUM(M7:M14)</f>
@@ -919,7 +919,7 @@
       </c>
       <c r="N6" s="9">
         <f>IF(M6&lt;&gt;0,L6/M6,0)</f>
-        <v>0.13274336283185842</v>
+        <v>0.24778761061946902</v>
       </c>
       <c r="P6" s="5" t="s">
         <v>13</v>
@@ -1045,13 +1045,15 @@
       <c r="K8" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="L8" s="8"/>
+      <c r="L8" s="8">
+        <v>13</v>
+      </c>
       <c r="M8" s="8">
         <v>15</v>
       </c>
       <c r="N8" s="9">
         <f t="shared" ref="N8:N14" si="5">IF(M8&lt;&gt;0,L8/M8,0)</f>
-        <v>0</v>
+        <v>0.8666666666666667</v>
       </c>
       <c r="P8" s="3" t="s">
         <v>51</v>

</xml_diff>

<commit_message>
discussion forum updates mostly
</commit_message>
<xml_diff>
--- a/grades.xlsx
+++ b/grades.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alf\Desktop\x86\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{356859F4-911F-4B55-BBE4-E1031596F08F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24E7E15D-D09F-4018-84A2-F002FBDB28E8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="7680" windowHeight="2580" xr2:uid="{BEB47269-8309-432F-A838-264E8E734028}"/>
   </bookViews>
@@ -627,7 +627,7 @@
   <dimension ref="A2:AC27"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="Q9" sqref="Q9"/>
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -845,7 +845,7 @@
       <c r="M5" s="13"/>
       <c r="N5" s="10">
         <f>N6*N2</f>
-        <v>0.1415929203539823</v>
+        <v>0.17840707964601771</v>
       </c>
       <c r="P5" s="5" t="s">
         <v>14</v>
@@ -854,7 +854,7 @@
       <c r="R5" s="13"/>
       <c r="S5" s="10">
         <f>S6*S2</f>
-        <v>0.2</v>
+        <v>0.18000000000000002</v>
       </c>
       <c r="U5" s="5" t="s">
         <v>14</v>
@@ -872,7 +872,7 @@
       <c r="AB5" s="13"/>
       <c r="AC5" s="10">
         <f>D5+I5+N5+S5+X5</f>
-        <v>0.42990359996563277</v>
+        <v>0.44671775925766821</v>
       </c>
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.25">
@@ -911,7 +911,7 @@
       </c>
       <c r="L6" s="8">
         <f>SUM(L7:L14)</f>
-        <v>50</v>
+        <v>63</v>
       </c>
       <c r="M6" s="8">
         <f>SUM(M7:M14)</f>
@@ -919,14 +919,14 @@
       </c>
       <c r="N6" s="9">
         <f>IF(M6&lt;&gt;0,L6/M6,0)</f>
-        <v>0.44247787610619471</v>
+        <v>0.55752212389380529</v>
       </c>
       <c r="P6" s="5" t="s">
         <v>13</v>
       </c>
       <c r="Q6" s="8">
         <f>SUM(Q7:Q8)</f>
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="R6" s="8">
         <f>SUM(R7:R8)</f>
@@ -934,7 +934,7 @@
       </c>
       <c r="S6" s="9">
         <f>IF(R6&lt;&gt;0,Q6/R6,0)</f>
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="U6" s="5" t="s">
         <v>13</v>
@@ -1061,14 +1061,14 @@
         <v>51</v>
       </c>
       <c r="Q8" s="8">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="R8" s="8">
         <v>70</v>
       </c>
       <c r="S8" s="9">
         <f>IF(R8&lt;&gt;0,Q8/R8,0)</f>
-        <v>1</v>
+        <v>0.8571428571428571</v>
       </c>
       <c r="U8" s="3" t="s">
         <v>51</v>
@@ -1192,13 +1192,15 @@
       <c r="K11" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="L11" s="8"/>
+      <c r="L11" s="8">
+        <v>13</v>
+      </c>
       <c r="M11" s="8">
         <v>13</v>
       </c>
       <c r="N11" s="9">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:29" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
sample final 1 done
Let's power through the rest of this today.
</commit_message>
<xml_diff>
--- a/grades.xlsx
+++ b/grades.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alf\Desktop\x86\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73C6FCF2-6F26-45B3-8EE4-05DFB225DF5C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2616523-1100-4216-842B-72B4434B9734}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="7680" windowHeight="2580" xr2:uid="{BEB47269-8309-432F-A838-264E8E734028}"/>
   </bookViews>
@@ -627,7 +627,7 @@
   <dimension ref="A2:AC27"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+      <selection activeCell="V7" sqref="V7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -827,7 +827,7 @@
       <c r="C5" s="13"/>
       <c r="D5" s="10">
         <f>D6*D2</f>
-        <v>7.5728155339805828E-2</v>
+        <v>0.1</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>14</v>
@@ -836,7 +836,7 @@
       <c r="H5" s="13"/>
       <c r="I5" s="10">
         <f>I6*I2</f>
-        <v>4.8000000000000001E-2</v>
+        <v>6.4000000000000001E-2</v>
       </c>
       <c r="K5" s="5" t="s">
         <v>14</v>
@@ -845,7 +845,7 @@
       <c r="M5" s="13"/>
       <c r="N5" s="10">
         <f>N6*N2</f>
-        <v>0.21805309734513273</v>
+        <v>0.29168141592920355</v>
       </c>
       <c r="P5" s="5" t="s">
         <v>14</v>
@@ -872,7 +872,7 @@
       <c r="AB5" s="13"/>
       <c r="AC5" s="10">
         <f>D5+I5+N5+S5+X5</f>
-        <v>0.52178125268493858</v>
+        <v>0.63568141592920357</v>
       </c>
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.25">
@@ -881,7 +881,7 @@
       </c>
       <c r="B6" s="8">
         <f>SUM(B7:B27)</f>
-        <v>156</v>
+        <v>206</v>
       </c>
       <c r="C6" s="8">
         <f>SUM(C7:C27)</f>
@@ -889,14 +889,14 @@
       </c>
       <c r="D6" s="9">
         <f>IF(C6&lt;&gt;0,B6/C6,0)</f>
-        <v>0.75728155339805825</v>
+        <v>1</v>
       </c>
       <c r="F6" s="5" t="s">
         <v>13</v>
       </c>
       <c r="G6" s="8">
         <f>SUM(G7:G16)</f>
-        <v>120</v>
+        <v>160</v>
       </c>
       <c r="H6" s="8">
         <f>SUM(H7:H16)</f>
@@ -904,14 +904,14 @@
       </c>
       <c r="I6" s="9">
         <f>IF(H6&lt;&gt;0,G6/H6,0)</f>
-        <v>0.6</v>
+        <v>0.8</v>
       </c>
       <c r="K6" s="5" t="s">
         <v>13</v>
       </c>
       <c r="L6" s="8">
         <f>SUM(L7:L14)</f>
-        <v>77</v>
+        <v>103</v>
       </c>
       <c r="M6" s="8">
         <f>SUM(M7:M14)</f>
@@ -919,7 +919,7 @@
       </c>
       <c r="N6" s="9">
         <f>IF(M6&lt;&gt;0,L6/M6,0)</f>
-        <v>0.68141592920353977</v>
+        <v>0.91150442477876104</v>
       </c>
       <c r="P6" s="5" t="s">
         <v>13</v>
@@ -1263,24 +1263,28 @@
       <c r="F13" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="G13" s="8"/>
+      <c r="G13" s="8">
+        <v>20</v>
+      </c>
       <c r="H13" s="8">
         <v>20</v>
       </c>
       <c r="I13" s="9">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K13" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="L13" s="8"/>
+      <c r="L13" s="8">
+        <v>13</v>
+      </c>
       <c r="M13" s="8">
         <v>14</v>
       </c>
       <c r="N13" s="9">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>0.9285714285714286</v>
       </c>
     </row>
     <row r="14" spans="1:29" x14ac:dyDescent="0.25">
@@ -1311,50 +1315,58 @@
       <c r="K14" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="L14" s="8"/>
+      <c r="L14" s="8">
+        <v>13</v>
+      </c>
       <c r="M14" s="8">
         <v>13</v>
       </c>
       <c r="N14" s="9">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="8"/>
+      <c r="B15" s="8">
+        <v>10</v>
+      </c>
       <c r="C15" s="8">
         <v>10</v>
       </c>
       <c r="D15" s="9">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F15" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="G15" s="8"/>
+      <c r="G15" s="8">
+        <v>20</v>
+      </c>
       <c r="H15" s="8">
         <v>20</v>
       </c>
       <c r="I15" s="9">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B16" s="8"/>
+      <c r="B16" s="8">
+        <v>10</v>
+      </c>
       <c r="C16" s="8">
         <v>10</v>
       </c>
       <c r="D16" s="9">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F16" s="3" t="s">
         <v>39</v>
@@ -1477,26 +1489,30 @@
       <c r="A24" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B24" s="8"/>
+      <c r="B24" s="8">
+        <v>10</v>
+      </c>
       <c r="C24" s="8">
         <v>10</v>
       </c>
       <c r="D24" s="9">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B25" s="8"/>
+      <c r="B25" s="8">
+        <v>10</v>
+      </c>
       <c r="C25" s="8">
         <v>10</v>
       </c>
       <c r="D25" s="9">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -1518,13 +1534,15 @@
       <c r="A27" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="8"/>
+      <c r="B27" s="8">
+        <v>10</v>
+      </c>
       <c r="C27" s="8">
         <v>10</v>
       </c>
       <c r="D27" s="9">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>